<commit_message>
Remove green markings from results
</commit_message>
<xml_diff>
--- a/results/Final_results.xlsx
+++ b/results/Final_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/493ecb1e13f02353/Unizeugs/Uni Ma/4_FSS2/Masterarbeit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3327" documentId="8_{324745AD-0062-4E42-A4BC-173C34805E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8627BB6-339B-46B2-B59F-C2FA451145B6}"/>
+  <xr:revisionPtr revIDLastSave="3330" documentId="8_{324745AD-0062-4E42-A4BC-173C34805E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{523FE636-D60A-41F9-927B-076990C572E7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{AB3301BC-916F-49D9-86FC-4CA2FAA690FC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{AB3301BC-916F-49D9-86FC-4CA2FAA690FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,12 +265,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -433,6 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,17 +446,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -806,29 +792,29 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46" t="s">
+      <c r="J1" s="47"/>
+      <c r="K1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="46"/>
+      <c r="L1" s="47"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
+      <c r="A2" s="47"/>
       <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
@@ -1159,51 +1145,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48" t="s">
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1650,37 +1636,37 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="49" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1861,25 +1847,25 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="49" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
@@ -1968,22 +1954,22 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2211,7 +2197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC1D46E-A54F-4AD2-AD0D-EC9B299836F5}">
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S60" sqref="S60"/>
     </sheetView>
   </sheetViews>
@@ -2223,32 +2209,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
     </row>
     <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
+      <c r="A2" s="49"/>
       <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
@@ -2266,7 +2252,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="48"/>
+      <c r="K2" s="49"/>
       <c r="L2" s="9" t="s">
         <v>32</v>
       </c>
@@ -2533,32 +2519,32 @@
       <c r="O9" s="24"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="47" t="s">
+      <c r="K10" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
@@ -2576,7 +2562,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="48"/>
+      <c r="K11" s="49"/>
       <c r="L11" s="9" t="s">
         <v>32</v>
       </c>
@@ -2890,32 +2876,32 @@
       <c r="O19" s="21"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
-      <c r="K20" s="47" t="s">
+      <c r="K20" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L20" s="50" t="s">
+      <c r="L20" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="9" t="s">
         <v>32</v>
       </c>
@@ -2933,7 +2919,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
-      <c r="K21" s="48"/>
+      <c r="K21" s="49"/>
       <c r="L21" s="9" t="s">
         <v>32</v>
       </c>
@@ -3189,32 +3175,32 @@
     </row>
     <row r="31" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
-      <c r="K34" s="47" t="s">
+      <c r="K34" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="50" t="s">
+      <c r="L34" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="51"/>
+      <c r="O34" s="51"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="9" t="s">
         <v>32</v>
       </c>
@@ -3232,7 +3218,7 @@
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="48"/>
+      <c r="K35" s="49"/>
       <c r="L35" s="9" t="s">
         <v>32</v>
       </c>
@@ -3504,32 +3490,32 @@
       <c r="O42" s="21"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
-      <c r="K43" s="47" t="s">
+      <c r="K43" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L43" s="50" t="s">
+      <c r="L43" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="M43" s="50"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="51"/>
+      <c r="O43" s="51"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="9" t="s">
         <v>32</v>
       </c>
@@ -3547,7 +3533,7 @@
       <c r="H44" s="21"/>
       <c r="I44" s="21"/>
       <c r="J44" s="21"/>
-      <c r="K44" s="48"/>
+      <c r="K44" s="49"/>
       <c r="L44" s="9" t="s">
         <v>32</v>
       </c>
@@ -3861,32 +3847,32 @@
       <c r="O52" s="21"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
       <c r="I53" s="21"/>
       <c r="J53" s="21"/>
-      <c r="K53" s="47" t="s">
+      <c r="K53" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="L53" s="50" t="s">
+      <c r="L53" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="M53" s="50"/>
-      <c r="N53" s="50"/>
-      <c r="O53" s="50"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="51"/>
+      <c r="O53" s="51"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="48"/>
+      <c r="A54" s="49"/>
       <c r="B54" s="9" t="s">
         <v>32</v>
       </c>
@@ -3904,7 +3890,7 @@
       <c r="H54" s="21"/>
       <c r="I54" s="21"/>
       <c r="J54" s="21"/>
-      <c r="K54" s="48"/>
+      <c r="K54" s="49"/>
       <c r="L54" s="9" t="s">
         <v>32</v>
       </c>
@@ -4289,18 +4275,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:O20"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="K53:K54"/>
@@ -4313,6 +4287,18 @@
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="K43:K44"/>
     <mergeCell ref="L43:O43"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4322,8 +4308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5E47C0-E45F-4DCC-BE10-48A4E43C96F5}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H36" activeCellId="6" sqref="D11 D23 H24 H12 H37 D35 H36"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4339,39 +4325,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -4669,7 +4655,7 @@
       <c r="A11" s="27"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="54"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="15"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -4680,43 +4666,40 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H12" s="56"/>
-    </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="48" t="s">
+      <c r="A14" s="48"/>
+      <c r="B14" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49" t="s">
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="9" t="s">
         <v>32</v>
       </c>
@@ -5014,7 +4997,7 @@
       <c r="A23" s="27"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="55"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="15"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -5025,43 +5008,40 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H24" s="56"/>
-    </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48" t="s">
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="48" t="s">
+      <c r="A26" s="48"/>
+      <c r="B26" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49" t="s">
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="9" t="s">
         <v>32</v>
       </c>
@@ -5354,22 +5334,17 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="56"/>
       <c r="H35" s="44" t="s">
         <v>53</v>
       </c>
       <c r="I35" s="44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H36" s="56"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>45</v>
       </c>
-      <c r="H37" s="56"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D43" s="24"/>
@@ -5388,21 +5363,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="F26:I26"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5413,7 +5388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB645DBB-1271-4BE3-B9B7-565494E5FF5E}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -5427,39 +5402,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -5722,7 +5697,6 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D10" s="56"/>
       <c r="H10" s="44" t="s">
         <v>51</v>
       </c>
@@ -5730,43 +5704,40 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="56"/>
-    </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48" t="s">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
@@ -6026,7 +5997,6 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D21" s="56"/>
       <c r="H21" s="44" t="s">
         <v>52</v>
       </c>
@@ -6035,43 +6005,40 @@
       </c>
       <c r="J21" s="33"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H22" s="56"/>
-    </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="48"/>
+      <c r="B24" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49" t="s">
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="9" t="s">
         <v>32</v>
       </c>
@@ -6331,7 +6298,6 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D32" s="56"/>
       <c r="H32" s="44" t="s">
         <v>53</v>
       </c>
@@ -6339,29 +6305,28 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:I24"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6369,9 +6334,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E86DBC-DF8D-406A-851F-9909E498D4BC}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:I2"/>
     </sheetView>
   </sheetViews>
@@ -6386,39 +6351,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -6678,7 +6643,6 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D10" s="56"/>
       <c r="H10" s="44" t="s">
         <v>51</v>
       </c>
@@ -6686,44 +6650,40 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="56"/>
-    </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48" t="s">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="51"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
@@ -6785,7 +6745,7 @@
       <c r="I15" s="24">
         <v>1794780000</v>
       </c>
-      <c r="J15" s="52"/>
+      <c r="J15" s="38"/>
       <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -6820,7 +6780,7 @@
         <f>3949588136-I15</f>
         <v>2154808136</v>
       </c>
-      <c r="J16" s="52"/>
+      <c r="J16" s="38"/>
       <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -6855,7 +6815,7 @@
         <f>3963536608-I16-I15</f>
         <v>13948472</v>
       </c>
-      <c r="J17" s="52"/>
+      <c r="J17" s="38"/>
       <c r="K17" s="38"/>
       <c r="M17">
         <v>1000</v>
@@ -6893,7 +6853,7 @@
         <f>6453261608-I17-I16-I15</f>
         <v>2489725000</v>
       </c>
-      <c r="J18" s="52"/>
+      <c r="J18" s="38"/>
       <c r="K18" s="38"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -6983,7 +6943,6 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D21" s="56"/>
       <c r="H21" s="44" t="s">
         <v>52</v>
       </c>
@@ -6991,43 +6950,40 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H22" s="56"/>
-    </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="48"/>
+      <c r="B24" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49" t="s">
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="9" t="s">
         <v>32</v>
       </c>
@@ -7287,7 +7243,6 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D32" s="56"/>
       <c r="H32" s="44" t="s">
         <v>53</v>
       </c>
@@ -7295,32 +7250,28 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="56"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F34" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:I24"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7330,7 +7281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCA2733-ABB7-485A-9458-633F2655D0F1}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E37" sqref="E37:E42"/>
     </sheetView>
   </sheetViews>
@@ -7344,39 +7295,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -7671,7 +7622,6 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D11" s="56"/>
       <c r="H11" s="44" t="s">
         <v>51</v>
       </c>
@@ -7681,42 +7631,42 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G12" s="33"/>
-      <c r="H12" s="57"/>
+      <c r="H12" s="45"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="48" t="s">
+      <c r="A14" s="48"/>
+      <c r="B14" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49" t="s">
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="9" t="s">
         <v>32</v>
       </c>
@@ -8011,7 +7961,6 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D23" s="56"/>
       <c r="H23" s="44" t="s">
         <v>52</v>
       </c>
@@ -8019,43 +7968,40 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H24" s="56"/>
-    </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48" t="s">
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="48" t="s">
+      <c r="A26" s="48"/>
+      <c r="B26" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49" t="s">
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="9" t="s">
         <v>32</v>
       </c>
@@ -8321,7 +8267,7 @@
         <v>48444569847</v>
       </c>
       <c r="F34" s="11">
-        <f t="shared" ref="B34:I34" si="14">SUM(F28:F33)</f>
+        <f t="shared" ref="F34:I34" si="14">SUM(F28:F33)</f>
         <v>19163815</v>
       </c>
       <c r="G34" s="11">
@@ -8346,7 +8292,6 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="56"/>
       <c r="H35" s="44" t="s">
         <v>53</v>
       </c>
@@ -8358,7 +8303,7 @@
       <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="H36" s="57"/>
+      <c r="H36" s="45"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
@@ -8402,7 +8347,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" activeCellId="1" sqref="D21 D10"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8416,39 +8361,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -8708,7 +8653,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D10" s="53"/>
+      <c r="D10" s="52"/>
       <c r="H10" s="44" t="s">
         <v>51</v>
       </c>
@@ -8717,42 +8662,42 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="53"/>
+      <c r="H11" s="52"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48" t="s">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
@@ -9012,7 +8957,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D21" s="53"/>
+      <c r="D21" s="52"/>
       <c r="H21" s="44" t="s">
         <v>52</v>
       </c>
@@ -9021,42 +8966,42 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H22" s="53"/>
+      <c r="H22" s="52"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="48"/>
+      <c r="B24" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49" t="s">
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="9" t="s">
         <v>32</v>
       </c>
@@ -9317,7 +9262,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D32" s="53"/>
+      <c r="D32" s="52"/>
       <c r="H32" s="44" t="s">
         <v>53</v>
       </c>
@@ -9329,25 +9274,25 @@
       <c r="B33" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="53"/>
+      <c r="H33" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:I24"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9357,8 +9302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191CE769-F988-4185-8A03-81D2E3BE8DAF}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9372,39 +9317,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -9658,13 +9603,13 @@
         <f>H9-H8+J8</f>
         <v>372019.92</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="53">
         <f>I9-I8+K8</f>
         <v>419837004187</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D10" s="53"/>
+      <c r="D10" s="52"/>
       <c r="H10" s="17" t="s">
         <v>51</v>
       </c>
@@ -9673,42 +9618,42 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="53"/>
+      <c r="H11" s="52"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48" t="s">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
@@ -9968,7 +9913,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D21" s="53"/>
+      <c r="D21" s="52"/>
       <c r="H21" s="44" t="s">
         <v>52</v>
       </c>
@@ -9977,42 +9922,42 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H22" s="53"/>
+      <c r="H22" s="52"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="48"/>
+      <c r="B24" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49" t="s">
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="9" t="s">
         <v>32</v>
       </c>
@@ -10272,7 +10217,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D32" s="53"/>
+      <c r="D32" s="52"/>
       <c r="H32" s="44" t="s">
         <v>53</v>
       </c>
@@ -10284,25 +10229,25 @@
       <c r="B33" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="53"/>
+      <c r="H33" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:I24"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10327,51 +10272,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48" t="s">
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
@@ -10676,27 +10621,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="9" t="s">
         <v>32</v>
       </c>

</xml_diff>